<commit_message>
Updated day-12.xlsx: added practice sheet for data
</commit_message>
<xml_diff>
--- a/day-12.xlsx
+++ b/day-12.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA ANALYST 2025\EXCEL\day 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1194CE4B-5176-46BE-9A54-3A55EEE80BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CD5890-6233-4C1E-9A9E-C2DFD85ECF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="basic" sheetId="2" r:id="rId1"/>
+    <sheet name="basic" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="Vlookup" sheetId="14" r:id="rId2"/>
     <sheet name="Hlookup" sheetId="15" r:id="rId3"/>
+    <sheet name="Task1" sheetId="17" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="186">
   <si>
     <t>ARC</t>
   </si>
@@ -174,13 +175,433 @@
   </si>
   <si>
     <t>automotive sq, near tp road , 400001</t>
+  </si>
+  <si>
+    <t>5 Examples of V lookup and H Lookup</t>
+  </si>
+  <si>
+    <t>EX 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
+    <t>Vrinda</t>
+  </si>
+  <si>
+    <t>Sharan</t>
+  </si>
+  <si>
+    <t>Gopi</t>
+  </si>
+  <si>
+    <t>Kunti</t>
+  </si>
+  <si>
+    <t>Arjun</t>
+  </si>
+  <si>
+    <t>Abhimanyu</t>
+  </si>
+  <si>
+    <t>Bhishma</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Unit test1</t>
+  </si>
+  <si>
+    <t>Unit test 2</t>
+  </si>
+  <si>
+    <t>Final test</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Vlookup</t>
+  </si>
+  <si>
+    <t>Final Test</t>
+  </si>
+  <si>
+    <t>EX 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department </t>
+  </si>
+  <si>
+    <t>Smith J</t>
+  </si>
+  <si>
+    <t>Edison</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex </t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Ex 3)</t>
+  </si>
+  <si>
+    <t>Procduct ID</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Usb cable</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Wireless mouse</t>
+  </si>
+  <si>
+    <t>computer</t>
+  </si>
+  <si>
+    <t>P01</t>
+  </si>
+  <si>
+    <t>P02</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>P04</t>
+  </si>
+  <si>
+    <t>P05</t>
+  </si>
+  <si>
+    <t>P06</t>
+  </si>
+  <si>
+    <t>P07</t>
+  </si>
+  <si>
+    <t>P08</t>
+  </si>
+  <si>
+    <t>P09</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Ex 4)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>EMP01</t>
+  </si>
+  <si>
+    <t>EMP02</t>
+  </si>
+  <si>
+    <t>EMP03</t>
+  </si>
+  <si>
+    <t>EMP04</t>
+  </si>
+  <si>
+    <t>EMP05</t>
+  </si>
+  <si>
+    <t>EMP06</t>
+  </si>
+  <si>
+    <t>EMP07</t>
+  </si>
+  <si>
+    <t>Kimi</t>
+  </si>
+  <si>
+    <t>Jinny</t>
+  </si>
+  <si>
+    <t>Kaka</t>
+  </si>
+  <si>
+    <t>Riya</t>
+  </si>
+  <si>
+    <t>Amit</t>
+  </si>
+  <si>
+    <t>Zubeen</t>
+  </si>
+  <si>
+    <t>shami</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Ex 5)</t>
+  </si>
+  <si>
+    <t>Subjects</t>
+  </si>
+  <si>
+    <t>Total marks</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>Raghav</t>
+  </si>
+  <si>
+    <t>Shaman</t>
+  </si>
+  <si>
+    <t>Sudeep</t>
+  </si>
+  <si>
+    <t>Sci</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Hlookup</t>
+  </si>
+  <si>
+    <t>Ex 1)</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Apples</t>
+  </si>
+  <si>
+    <t>Kiwis</t>
+  </si>
+  <si>
+    <t>Ex 2)</t>
+  </si>
+  <si>
+    <t>Hindi</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Tina</t>
+  </si>
+  <si>
+    <t>Neha</t>
+  </si>
+  <si>
+    <t>Anandi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kumar </t>
+  </si>
+  <si>
+    <t>Date/Div</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Shyam</t>
+  </si>
+  <si>
+    <t>Sugam</t>
+  </si>
+  <si>
+    <t>Adarsh</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>Ex 5 )</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Pens</t>
+  </si>
+  <si>
+    <t>Pencils</t>
+  </si>
+  <si>
+    <t>Sketch pens</t>
+  </si>
+  <si>
+    <t>Crayons</t>
+  </si>
+  <si>
+    <t>Chart paper</t>
+  </si>
+  <si>
+    <t>A2 copies</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Pineapple</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,8 +609,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +704,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -266,7 +750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -280,6 +764,52 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A40DD5A-2EA0-453B-B205-8D25B7B6EF10}">
   <dimension ref="D4:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="I2" zoomScale="103" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,7 +1486,7 @@
   <dimension ref="D6:J18"/>
   <sheetViews>
     <sheetView topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1212,4 +1742,1548 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DD68F6-68DC-4782-B697-481032ED6758}">
+  <dimension ref="A1:R123"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="102" workbookViewId="0">
+      <selection activeCell="N67" sqref="N67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="I1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+    </row>
+    <row r="2" spans="1:16" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K2" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="13">
+        <v>16</v>
+      </c>
+      <c r="F5" s="13">
+        <v>10</v>
+      </c>
+      <c r="G5" s="13">
+        <v>84</v>
+      </c>
+      <c r="H5" s="13">
+        <v>87</v>
+      </c>
+      <c r="I5" s="13">
+        <v>89</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="N5" s="17">
+        <f>VLOOKUP(M5,$C$4:$I$11,7,FALSE)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C6" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="13">
+        <v>17</v>
+      </c>
+      <c r="F6" s="13">
+        <v>9</v>
+      </c>
+      <c r="G6" s="13">
+        <v>95</v>
+      </c>
+      <c r="H6" s="13">
+        <v>93</v>
+      </c>
+      <c r="I6" s="13">
+        <v>79</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="17">
+        <f t="shared" ref="N6:N9" si="0">VLOOKUP(M6,$C$4:$I$11,7,FALSE)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="13">
+        <v>15</v>
+      </c>
+      <c r="F7" s="13">
+        <v>20</v>
+      </c>
+      <c r="G7" s="13">
+        <v>85</v>
+      </c>
+      <c r="H7" s="13">
+        <v>78</v>
+      </c>
+      <c r="I7" s="13">
+        <v>85</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="17">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="13">
+        <v>14</v>
+      </c>
+      <c r="F8" s="13">
+        <v>8</v>
+      </c>
+      <c r="G8" s="13">
+        <v>92</v>
+      </c>
+      <c r="H8" s="13">
+        <v>80</v>
+      </c>
+      <c r="I8" s="13">
+        <v>79</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="17">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="13">
+        <v>15</v>
+      </c>
+      <c r="F9" s="13">
+        <v>10</v>
+      </c>
+      <c r="G9" s="13">
+        <v>88</v>
+      </c>
+      <c r="H9" s="13">
+        <v>65</v>
+      </c>
+      <c r="I9" s="13">
+        <v>80</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="17">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="13">
+        <v>16</v>
+      </c>
+      <c r="F10" s="13">
+        <v>9</v>
+      </c>
+      <c r="G10" s="13">
+        <v>90</v>
+      </c>
+      <c r="H10" s="13">
+        <v>89</v>
+      </c>
+      <c r="I10" s="13">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="13">
+        <v>15</v>
+      </c>
+      <c r="F11" s="13">
+        <v>9</v>
+      </c>
+      <c r="G11" s="13">
+        <v>63</v>
+      </c>
+      <c r="H11" s="13">
+        <v>78</v>
+      </c>
+      <c r="I11" s="13">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M15" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="M16" s="18">
+        <v>104</v>
+      </c>
+      <c r="N16" s="18" t="str">
+        <f>VLOOKUP(M16,$C$16:$E$21,3,FALSE)</f>
+        <v>HR</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C17" s="13">
+        <v>101</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17" s="18">
+        <v>102</v>
+      </c>
+      <c r="N17" s="18" t="str">
+        <f t="shared" ref="N17:N19" si="1">VLOOKUP(M17,$C$16:$E$21,3,FALSE)</f>
+        <v>Finance</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C18" s="13">
+        <v>102</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" s="18">
+        <v>101</v>
+      </c>
+      <c r="N18" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>HR</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C19" s="13">
+        <v>103</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" s="18">
+        <v>103</v>
+      </c>
+      <c r="N19" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>Sales</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C20" s="13">
+        <v>104</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C21" s="13">
+        <v>105</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="M26" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="N26" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C27" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="17">
+        <v>230</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="N27" s="13">
+        <f>VLOOKUP(M27,$C$26:$E$35,3,FALSE)</f>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C28" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="17">
+        <v>300</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="N28" s="13">
+        <f t="shared" ref="N28:N31" si="2">VLOOKUP(M28,$C$26:$E$35,3,FALSE)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C29" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="17">
+        <v>153</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="N29" s="13">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C30" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="17">
+        <v>250</v>
+      </c>
+      <c r="M30" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="N30" s="13">
+        <f t="shared" si="2"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C31" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="17">
+        <v>380</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="N31" s="13">
+        <f t="shared" si="2"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C32" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="17">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C33" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="17">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C34" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C35" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="17">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="N41" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C42" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G42" s="17">
+        <v>40000</v>
+      </c>
+      <c r="M42" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="N42" s="17">
+        <f>VLOOKUP(M42,$D$41:$G$48,4,FALSE)</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C43" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G43" s="17">
+        <v>50000</v>
+      </c>
+      <c r="M43" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="N43" s="17">
+        <f t="shared" ref="N43:N46" si="3">VLOOKUP(M43,$D$41:$G$48,4,FALSE)</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C44" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="17">
+        <v>20000</v>
+      </c>
+      <c r="M44" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="N44" s="17">
+        <f t="shared" si="3"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C45" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G45" s="17">
+        <v>10000</v>
+      </c>
+      <c r="M45" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="N45" s="17">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C46" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46" s="17">
+        <v>60000</v>
+      </c>
+      <c r="M46" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="N46" s="17">
+        <f t="shared" si="3"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C47" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G47" s="17">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C48" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G48" s="17">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="M55" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="N55" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C56" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="17">
+        <v>60</v>
+      </c>
+      <c r="M56" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="N56" s="17">
+        <f>VLOOKUP(M56,$C$55:$E$60,3,FALSE)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C57" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" s="17">
+        <v>70</v>
+      </c>
+      <c r="M57" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="N57" s="17">
+        <f t="shared" ref="N57:N58" si="4">VLOOKUP(M57,$C$55:$E$60,3,FALSE)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C58" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="17">
+        <v>60</v>
+      </c>
+      <c r="M58" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="N58" s="17">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C59" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E59" s="17">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C60" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60" s="17">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="K64" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="26"/>
+      <c r="M67" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="N67" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C68" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="D68" s="17">
+        <v>34</v>
+      </c>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="M68" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="N68" s="16">
+        <f>HLOOKUP(M68,C67:D71,4,FALSE)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C69" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="D69" s="17">
+        <v>234</v>
+      </c>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+    </row>
+    <row r="70" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C70" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D70" s="17">
+        <v>45</v>
+      </c>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="26"/>
+    </row>
+    <row r="71" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C71" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D71" s="29">
+        <v>343</v>
+      </c>
+      <c r="E71" s="27"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="27"/>
+    </row>
+    <row r="76" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G76" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="M76" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="N76" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="O76" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="P76" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q76" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C77" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D77" s="17">
+        <v>45</v>
+      </c>
+      <c r="E77" s="17">
+        <v>98</v>
+      </c>
+      <c r="F77" s="17">
+        <v>57</v>
+      </c>
+      <c r="G77" s="17">
+        <f>SUM(D77,E77,F77)</f>
+        <v>200</v>
+      </c>
+      <c r="M77" s="16" t="str">
+        <f>HLOOKUP(M76,C76:G81,3,FALSE)</f>
+        <v>Tina</v>
+      </c>
+      <c r="N77" s="16">
+        <f t="shared" ref="N77:Q77" si="5">HLOOKUP(N76,D76:H81,3,FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="O77" s="16">
+        <f t="shared" si="5"/>
+        <v>67</v>
+      </c>
+      <c r="P77" s="16">
+        <f t="shared" si="5"/>
+        <v>68</v>
+      </c>
+      <c r="Q77" s="16">
+        <f t="shared" si="5"/>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C78" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D78" s="17">
+        <v>76</v>
+      </c>
+      <c r="E78" s="17">
+        <v>67</v>
+      </c>
+      <c r="F78" s="17">
+        <v>68</v>
+      </c>
+      <c r="G78" s="17">
+        <f t="shared" ref="G78:G81" si="6">SUM(D78,E78,F78)</f>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C79" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D79" s="17">
+        <v>56</v>
+      </c>
+      <c r="E79" s="17">
+        <v>87</v>
+      </c>
+      <c r="F79" s="17">
+        <v>78</v>
+      </c>
+      <c r="G79" s="17">
+        <f t="shared" si="6"/>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C80" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D80" s="17">
+        <v>67</v>
+      </c>
+      <c r="E80" s="17">
+        <v>87</v>
+      </c>
+      <c r="F80" s="17">
+        <v>89</v>
+      </c>
+      <c r="G80" s="17">
+        <f t="shared" si="6"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C81" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D81" s="17">
+        <v>56</v>
+      </c>
+      <c r="E81" s="17">
+        <v>67</v>
+      </c>
+      <c r="F81" s="17">
+        <v>37</v>
+      </c>
+      <c r="G81" s="17">
+        <f t="shared" si="6"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C87" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D87" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F87" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="G87" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H87" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="M87" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="N87" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="O87" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="P87" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q87" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="R87" s="19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C88" s="23">
+        <v>45658</v>
+      </c>
+      <c r="D88" s="17">
+        <v>45</v>
+      </c>
+      <c r="E88" s="17">
+        <v>56</v>
+      </c>
+      <c r="F88" s="17">
+        <v>56</v>
+      </c>
+      <c r="G88" s="17">
+        <v>8</v>
+      </c>
+      <c r="H88" s="17">
+        <v>45</v>
+      </c>
+      <c r="M88" s="21">
+        <v>45664</v>
+      </c>
+      <c r="N88" s="16">
+        <f t="shared" ref="N88:R88" si="7">HLOOKUP(N87,D87:I96,8,FALSE)</f>
+        <v>56</v>
+      </c>
+      <c r="O88" s="16">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="P88" s="16">
+        <f t="shared" si="7"/>
+        <v>43</v>
+      </c>
+      <c r="Q88" s="16">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="R88" s="16">
+        <f t="shared" si="7"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C89" s="23">
+        <v>45659</v>
+      </c>
+      <c r="D89" s="17">
+        <v>67</v>
+      </c>
+      <c r="E89" s="17">
+        <v>87</v>
+      </c>
+      <c r="F89" s="17">
+        <v>56</v>
+      </c>
+      <c r="G89" s="17">
+        <v>67</v>
+      </c>
+      <c r="H89" s="17">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C90" s="23">
+        <v>45660</v>
+      </c>
+      <c r="D90" s="17">
+        <v>45</v>
+      </c>
+      <c r="E90" s="17">
+        <v>75</v>
+      </c>
+      <c r="F90" s="17">
+        <v>45</v>
+      </c>
+      <c r="G90" s="17">
+        <v>4</v>
+      </c>
+      <c r="H90" s="17">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C91" s="23">
+        <v>45661</v>
+      </c>
+      <c r="D91" s="17">
+        <v>68</v>
+      </c>
+      <c r="E91" s="17">
+        <v>6</v>
+      </c>
+      <c r="F91" s="17">
+        <v>67</v>
+      </c>
+      <c r="G91" s="17">
+        <v>65</v>
+      </c>
+      <c r="H91" s="17">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C92" s="23">
+        <v>45662</v>
+      </c>
+      <c r="D92" s="17">
+        <v>78</v>
+      </c>
+      <c r="E92" s="17">
+        <v>34</v>
+      </c>
+      <c r="F92" s="17">
+        <v>67</v>
+      </c>
+      <c r="G92" s="17">
+        <v>5</v>
+      </c>
+      <c r="H92" s="17">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C93" s="23">
+        <v>45663</v>
+      </c>
+      <c r="D93" s="17">
+        <v>67</v>
+      </c>
+      <c r="E93" s="17">
+        <v>45</v>
+      </c>
+      <c r="F93" s="17">
+        <v>45</v>
+      </c>
+      <c r="G93" s="17">
+        <v>56</v>
+      </c>
+      <c r="H93" s="17">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C94" s="23">
+        <v>45664</v>
+      </c>
+      <c r="D94" s="17">
+        <v>56</v>
+      </c>
+      <c r="E94" s="17">
+        <v>6</v>
+      </c>
+      <c r="F94" s="17">
+        <v>43</v>
+      </c>
+      <c r="G94" s="17">
+        <v>45</v>
+      </c>
+      <c r="H94" s="17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C95" s="23">
+        <v>45665</v>
+      </c>
+      <c r="D95" s="17">
+        <v>79</v>
+      </c>
+      <c r="E95" s="17">
+        <v>45</v>
+      </c>
+      <c r="F95" s="17">
+        <v>8</v>
+      </c>
+      <c r="G95" s="17">
+        <v>67</v>
+      </c>
+      <c r="H95" s="17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C96" s="23">
+        <v>45666</v>
+      </c>
+      <c r="D96" s="17">
+        <v>80</v>
+      </c>
+      <c r="E96" s="17">
+        <v>87</v>
+      </c>
+      <c r="F96" s="17">
+        <v>78</v>
+      </c>
+      <c r="G96" s="17">
+        <v>98</v>
+      </c>
+      <c r="H96" s="17">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A103" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E103" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="F103" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G103" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="M103" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="N103" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C104" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="D104" s="16">
+        <v>14983</v>
+      </c>
+      <c r="E104" s="16">
+        <v>14975</v>
+      </c>
+      <c r="F104" s="16">
+        <v>44663</v>
+      </c>
+      <c r="G104" s="16">
+        <v>23445</v>
+      </c>
+      <c r="M104" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="N104" s="17">
+        <f>HLOOKUP(M104,C103:G110,5,FALSE)</f>
+        <v>13455</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C105" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="D105" s="16">
+        <v>14093</v>
+      </c>
+      <c r="E105" s="16">
+        <v>13453</v>
+      </c>
+      <c r="F105" s="16">
+        <v>24566</v>
+      </c>
+      <c r="G105" s="16">
+        <v>23454</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C106" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D106" s="16">
+        <v>13094</v>
+      </c>
+      <c r="E106" s="16">
+        <v>24566</v>
+      </c>
+      <c r="F106" s="16">
+        <v>24554</v>
+      </c>
+      <c r="G106" s="16">
+        <v>34234</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C107" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D107" s="16">
+        <v>15032</v>
+      </c>
+      <c r="E107" s="16">
+        <v>13455</v>
+      </c>
+      <c r="F107" s="16">
+        <v>24542</v>
+      </c>
+      <c r="G107" s="16">
+        <v>23434</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C108" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="D108" s="16">
+        <v>15934</v>
+      </c>
+      <c r="E108" s="16">
+        <v>25656</v>
+      </c>
+      <c r="F108" s="16">
+        <v>34565</v>
+      </c>
+      <c r="G108" s="16">
+        <v>23455</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C109" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D109" s="16">
+        <v>15034</v>
+      </c>
+      <c r="E109" s="16">
+        <v>35677</v>
+      </c>
+      <c r="F109" s="16">
+        <v>45664</v>
+      </c>
+      <c r="G109" s="16">
+        <v>34655</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C110" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D110" s="16">
+        <v>15934</v>
+      </c>
+      <c r="E110" s="16">
+        <v>54664</v>
+      </c>
+      <c r="F110" s="16">
+        <v>24566</v>
+      </c>
+      <c r="G110" s="16">
+        <v>23454</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A116" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C116" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D116" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="E116" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="M116" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="N116" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C117" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D117" s="16">
+        <v>500</v>
+      </c>
+      <c r="E117" s="25">
+        <v>346547</v>
+      </c>
+      <c r="M117" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="N117" s="16">
+        <f>HLOOKUP(M117,C116:E123,3,FALSE)</f>
+        <v>55645</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C118" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="D118" s="16">
+        <v>300</v>
+      </c>
+      <c r="E118" s="25">
+        <v>55645</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C119" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="D119" s="16">
+        <v>433</v>
+      </c>
+      <c r="E119" s="25">
+        <v>34545</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C120" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D120" s="16">
+        <v>356</v>
+      </c>
+      <c r="E120" s="25">
+        <v>6753</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C121" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D121" s="16">
+        <v>345</v>
+      </c>
+      <c r="E121" s="25">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C122" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D122" s="16">
+        <v>564</v>
+      </c>
+      <c r="E122" s="25">
+        <v>3456</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C123" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D123" s="16">
+        <v>345</v>
+      </c>
+      <c r="E123" s="25">
+        <v>78678</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>